<commit_message>
Tests for checking time of calculations for bigger input files filled with fake generated data
</commit_message>
<xml_diff>
--- a/src/main/resources/optimizationTasksData/JMatPro/microAlloy/info/ModelSzeligaDane38MnSV4Poprawiony.xlsx
+++ b/src/main/resources/optimizationTasksData/JMatPro/microAlloy/info/ModelSzeligaDane38MnSV4Poprawiony.xlsx
@@ -29,7 +29,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'stress-strain'!$T$63</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'stress-strain'!$T$64</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
@@ -459,234 +459,384 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'stress-strain'!$Q$3:$Q$38</c:f>
+              <c:f>'stress-strain'!$Q$3:$Q$63</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="61"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.12</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.14000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.22</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.24</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.26</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>0.32</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.34</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>0.36</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.38</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>0.44</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>0.46</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>1.3</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'stress-strain'!$R$3:$R$38</c:f>
+              <c:f>'stress-strain'!$R$3:$R$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="61"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>230.55719999999999</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>249.4804</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>261.37470000000002</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>270.1891</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>277.24439999999998</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>283.15320000000003</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>288.25150000000002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>291.99400000000003</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>291.93689999999998</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>291.85809999999998</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>291.75209999999998</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>291.61669999999998</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>291.44920000000002</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>291.24740000000003</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>291.01069999999999</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>290.73439999999999</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>290.4187</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>290.07139999999998</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>289.6884</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>289.27229999999997</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>288.8331</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>288.36279999999999</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>287.88170000000002</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>287.36669999999998</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>286.8544</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>284.1146</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>281.33589999999998</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>278.65370000000001</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>276.11020000000002</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>273.72609999999997</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>271.4889</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>269.40100000000001</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>267.4479</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>265.61750000000001</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>263.90519999999998</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>262.2679</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>260.73930000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>259.27969999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>257.91379999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>256.59030000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>255.33779999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>254.14789999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>253.0121</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>251.92359999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>250.87530000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>249.8673</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>248.8998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>247.96260000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>247.05719999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>246.18350000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>245.3408</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>244.52930000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>243.74959999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>242.9897</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>242.24029999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>241.52199999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>240.83629999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>240.14940000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>239.48609999999999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>238.85749999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -707,236 +857,391 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'stress-strain'!$Q$3:$Q$38</c:f>
+              <c:f>'stress-strain'!$Q$3:$Q$63</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="61"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.12</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.14000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.22</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.24</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.26</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>0.32</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.34</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>0.36</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.38</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>0.44</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>0.46</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>1.3</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>1.4</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'stress-strain'!$S$3:$S$38</c:f>
+              <c:f>'stress-strain'!$S$3:$S$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>249.2330959988295</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>261.61032746398615</c:v>
+                  <c:v>230.5572182791816</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>268.69479836240151</c:v>
+                  <c:v>251.16500908383895</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>273.52522730180021</c:v>
+                  <c:v>263.10410186919728</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>277.08774219986981</c:v>
+                  <c:v>271.12608338564445</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>279.83212843609181</c:v>
+                  <c:v>276.86050732958114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>282.00280251715759</c:v>
+                  <c:v>281.08502683017429</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>283.74792963960653</c:v>
+                  <c:v>284.23921728284932</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>285.16436486749222</c:v>
+                  <c:v>286.59896475831698</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>286.31902865926725</c:v>
+                  <c:v>288.35018107338431</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>287.26016626965634</c:v>
+                  <c:v>289.62473022914895</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>288.02375081427164</c:v>
+                  <c:v>290.51980048686238</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>288.63734915917053</c:v>
+                  <c:v>291.109174733131</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>289.12257107575414</c:v>
+                  <c:v>291.45018865093266</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>289.49668355192915</c:v>
+                  <c:v>291.58823686845068</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>289.77371075464004</c:v>
+                  <c:v>291.55980814685705</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>289.96520499937429</c:v>
+                  <c:v>291.39459814759186</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>290.08080044079816</c:v>
+                  <c:v>291.11702174845163</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>290.12861923806435</c:v>
+                  <c:v>290.74732181536058</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>290.11557510444641</c:v>
+                  <c:v>290.30239917134031</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>290.04760394262308</c:v>
+                  <c:v>289.79644524143504</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>289.92984168041551</c:v>
+                  <c:v>289.24143204036159</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>289.76676322021029</c:v>
+                  <c:v>288.64749706072621</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>289.56229230960747</c:v>
+                  <c:v>288.02324941620788</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>289.31988936566091</c:v>
+                  <c:v>287.37601608634117</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>287.63550067687703</c:v>
+                  <c:v>286.71204197286318</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>285.35004588911443</c:v>
+                  <c:v>283.30235363563509</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>282.63882253169038</c:v>
+                  <c:v>280.01094271643501</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>279.6168804963234</c:v>
+                  <c:v>277.02751904406716</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>276.36391188030075</c:v>
+                  <c:v>274.41755069974454</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>272.93742135852062</c:v>
+                  <c:v>272.18489093075505</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>269.38025021244636</c:v>
+                  <c:v>270.30391816760095</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>265.72513982113162</c:v>
+                  <c:v>268.73652053929567</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>261.99763605408333</c:v>
+                  <c:v>267.44110282690588</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>258.21801246650381</c:v>
+                  <c:v>266.37724352284613</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>254.40258678226894</c:v>
+                  <c:v>265.50793732816174</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>264.80049502256753</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>264.22670905139574</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>263.76263459311076</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>263.38818760962107</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>263.08667477074783</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>262.84431900555984</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>262.64981415520498</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>262.49392438186777</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>262.36913367909739</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>262.26934506321521</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>262.18962600096256</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>262.1259952397748</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>262.07524577376159</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>262.03479878214819</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>262.00258376184746</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>261.97694058782798</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>261.95653978332768</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>261.94031781556856</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>261.92742472469661</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>261.91718183222912</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>261.90904765716965</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>261.90259049492767</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>261.89746639062406</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>261.8934014698284</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>261.89017778206465</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,11 +1258,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91185536"/>
-        <c:axId val="91187072"/>
+        <c:axId val="104747392"/>
+        <c:axId val="104748928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91185536"/>
+        <c:axId val="104747392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -984,7 +1289,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91187072"/>
+        <c:crossAx val="104748928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -992,7 +1297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91187072"/>
+        <c:axId val="104748928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1325,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91185536"/>
+        <c:crossAx val="104747392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1471,7 +1776,7 @@
   <dimension ref="A1:AL141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1693,50 +1998,50 @@
         <v>15.6092</v>
       </c>
       <c r="Q3" s="34">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="R3" s="7">
-        <v>230.55719999999999</v>
+        <v>0</v>
       </c>
       <c r="S3" s="24">
         <f t="shared" ref="S3:S34" si="0">SQRT(3)*(U3*$X$14*(Q3^$X$15)*EXP($X$16/$Q$1)+(1-U3)*$X$17*EXP($X$18/$Q$1))*(SQRT(3)*$AA$11)^$X$19</f>
-        <v>249.2330959988295</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T62" si="1">SQRT((R3-S3)^2)</f>
-        <v>18.675895998829503</v>
+        <f t="shared" ref="T3" si="1">SQRT((R3-S3)^2)</f>
+        <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U62" si="2">EXP(-$X$13*Q3)</f>
-        <v>0.99629183622638262</v>
+        <f t="shared" ref="U3" si="2">EXP(-$X$13*Q3)</f>
+        <v>1</v>
       </c>
       <c r="W3">
         <f>SQRT(3)</f>
         <v>1.7320508075688772</v>
       </c>
       <c r="X3">
-        <f>U3*$X$14</f>
-        <v>15.128942941924597</v>
+        <f>U4*$X$14</f>
+        <v>8.4552343437227648</v>
       </c>
       <c r="Y3" s="33">
-        <f>(Q3^$X$15)</f>
-        <v>0.74390411518408206</v>
+        <f>(Q4^$X$15)</f>
+        <v>0.60851341662203329</v>
       </c>
       <c r="Z3">
         <f>EXP($X$16/$Q$1)</f>
-        <v>0.99984465269377565</v>
+        <v>1.0182013040318949</v>
       </c>
       <c r="AA3">
-        <f>(1-U3)*$X$17</f>
-        <v>-2.9452355286683808E-3</v>
+        <f>(1-U4)*$X$17</f>
+        <v>0.30012700237410189</v>
       </c>
       <c r="AB3">
         <f>EXP($X$18/$Q$1)</f>
-        <v>1.0001429237460637</v>
+        <v>0.98458942149611484</v>
       </c>
       <c r="AC3">
         <f>(SQRT(3)*$AA$11)^$X$19</f>
-        <v>12.790888461026006</v>
+        <v>24.052348552153074</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
@@ -1789,36 +2094,36 @@
         <v>17.1952</v>
       </c>
       <c r="Q4" s="34">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="R4" s="7">
-        <v>249.4804</v>
+        <v>230.55719999999999</v>
       </c>
       <c r="S4" s="24">
         <f t="shared" si="0"/>
-        <v>261.61032746398615</v>
+        <v>230.5572182791816</v>
       </c>
       <c r="T4">
-        <f t="shared" si="1"/>
-        <v>12.129927463986149</v>
+        <f t="shared" ref="T4:T63" si="3">SQRT((R4-S4)^2)</f>
+        <v>1.8279181603020334E-5</v>
       </c>
       <c r="U4">
-        <f t="shared" si="2"/>
-        <v>0.99259742293133735</v>
+        <f t="shared" ref="U4:U63" si="4">EXP(-$X$13*Q4)</f>
+        <v>0.95299116208396883</v>
       </c>
       <c r="X4" s="31" t="s">
         <v>34</v>
       </c>
       <c r="Y4" s="33">
-        <f>U3*$X$14*(Q3^$X$15)</f>
-        <v>11.254482912882882</v>
+        <f>U4*$X$14*(Q4^$X$15)</f>
+        <v>5.1451235388386953</v>
       </c>
       <c r="AA4" s="28" t="s">
         <v>36</v>
       </c>
       <c r="AB4">
         <f>AA3*EXP($X$18/$Q$1)</f>
-        <v>-2.9456564727631781E-3</v>
+        <v>0.29550187164288005</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
@@ -1871,30 +2176,30 @@
         <v>21.003499999999999</v>
       </c>
       <c r="Q5" s="34">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="R5" s="7">
-        <v>261.37470000000002</v>
+        <v>249.4804</v>
       </c>
       <c r="S5" s="24">
         <f t="shared" si="0"/>
-        <v>268.69479836240151</v>
+        <v>251.16500908383895</v>
       </c>
       <c r="T5">
-        <f t="shared" si="1"/>
-        <v>7.3200983624014953</v>
+        <f t="shared" si="3"/>
+        <v>1.68460908383895</v>
       </c>
       <c r="U5">
-        <f t="shared" si="2"/>
-        <v>0.9889167091258374</v>
+        <f t="shared" si="4"/>
+        <v>0.90819215501015338</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="31" t="s">
         <v>35</v>
       </c>
       <c r="Z5" s="33">
-        <f>U3*$X$14*(Q3^$X$15)*EXP($X$16/$Q$1)</f>
-        <v>11.252734559279418</v>
+        <f>U4*$X$14*(Q4^$X$15)*EXP($X$16/$Q$1)</f>
+        <v>5.2387714966507577</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
@@ -1947,30 +2252,30 @@
         <v>27.9193</v>
       </c>
       <c r="Q6" s="34">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="R6" s="7">
-        <v>270.1891</v>
+        <v>261.37470000000002</v>
       </c>
       <c r="S6" s="24">
         <f t="shared" si="0"/>
-        <v>273.52522730180021</v>
+        <v>263.10410186919728</v>
       </c>
       <c r="T6">
-        <f t="shared" si="1"/>
-        <v>3.336127301800218</v>
+        <f t="shared" si="3"/>
+        <v>1.729401869197261</v>
       </c>
       <c r="U6">
-        <f t="shared" si="2"/>
-        <v>0.98524964400993209</v>
+        <f t="shared" si="4"/>
+        <v>0.86549909719867002</v>
       </c>
       <c r="X6" s="13"/>
       <c r="AA6" s="31" t="s">
         <v>37</v>
       </c>
       <c r="AB6">
-        <f>(U3*$X$14*(Q3^$X$15)*EXP($X$16/$Q$1)+(1-U3)*$X$17*EXP($X$18/$Q$1))</f>
-        <v>11.249788902806655</v>
+        <f>(U4*$X$14*(Q4^$X$15)*EXP($X$16/$Q$1)+(1-U4)*$X$17*EXP($X$18/$Q$1))</f>
+        <v>5.534273368293638</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
@@ -2023,29 +2328,29 @@
         <v>38.2378</v>
       </c>
       <c r="Q7" s="34">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="R7" s="7">
-        <v>277.24439999999998</v>
+        <v>270.1891</v>
       </c>
       <c r="S7" s="24">
         <f t="shared" si="0"/>
-        <v>277.08774219986981</v>
+        <v>271.12608338564445</v>
       </c>
       <c r="T7">
-        <f t="shared" si="1"/>
-        <v>0.15665780013017638</v>
+        <f t="shared" si="3"/>
+        <v>0.93698338564445294</v>
       </c>
       <c r="U7">
-        <f t="shared" si="2"/>
-        <v>0.98159617697204504</v>
+        <f t="shared" si="4"/>
+        <v>0.82481299042198641</v>
       </c>
       <c r="Z7" s="28" t="s">
         <v>38</v>
       </c>
       <c r="AA7">
-        <f>SQRT(3)*(U3*$X$14*(Q3^$X$15)*EXP($X$16/$Q$1)+(1-U3)*$X$17*EXP($X$18/$Q$1))</f>
-        <v>19.485205954085661</v>
+        <f>SQRT(3)*(U4*$X$14*(Q4^$X$15)*EXP($X$16/$Q$1)+(1-U4)*$X$17*EXP($X$18/$Q$1))</f>
+        <v>9.5856426568599264</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
@@ -2098,22 +2403,22 @@
         <v>51.304900000000004</v>
       </c>
       <c r="Q8" s="34">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="R8" s="7">
-        <v>283.15320000000003</v>
+        <v>277.24439999999998</v>
       </c>
       <c r="S8" s="24">
         <f t="shared" si="0"/>
-        <v>279.83212843609181</v>
+        <v>276.86050732958114</v>
       </c>
       <c r="T8">
-        <f t="shared" si="1"/>
-        <v>3.3210715639082196</v>
+        <f t="shared" si="3"/>
+        <v>0.38389267041884523</v>
       </c>
       <c r="U8">
-        <f t="shared" si="2"/>
-        <v>0.97795625758827609</v>
+        <f t="shared" si="4"/>
+        <v>0.78603949024420228</v>
       </c>
       <c r="X8" s="9"/>
       <c r="Y8" s="9"/>
@@ -2121,8 +2426,8 @@
         <v>39</v>
       </c>
       <c r="AC8" s="32">
-        <f>SQRT(3)*(U3*$X$14*(Q3^$X$15)*EXP($X$16/$Q$1)+(1-U3)*$X$17*EXP($X$18/$Q$1))*(SQRT(3)*$AA$11)^$X$19</f>
-        <v>249.2330959988295</v>
+        <f>SQRT(3)*(U4*$X$14*(Q4^$X$15)*EXP($X$16/$Q$1)+(1-U4)*$X$17*EXP($X$18/$Q$1))*(SQRT(3)*$AA$11)^$X$19</f>
+        <v>230.5572182791816</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
@@ -2175,22 +2480,22 @@
         <v>65.676400000000001</v>
       </c>
       <c r="Q9" s="34">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="R9" s="7">
-        <v>288.25150000000002</v>
+        <v>283.15320000000003</v>
       </c>
       <c r="S9" s="24">
         <f t="shared" si="0"/>
-        <v>282.00280251715759</v>
+        <v>281.08502683017429</v>
       </c>
       <c r="T9">
-        <f t="shared" si="1"/>
-        <v>6.2486974828424309</v>
+        <f t="shared" si="3"/>
+        <v>2.0681731698257408</v>
       </c>
       <c r="U9">
-        <f t="shared" si="2"/>
-        <v>0.97432983562170483</v>
+        <f t="shared" si="4"/>
+        <v>0.74908868725171285</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
@@ -2243,22 +2548,22 @@
         <v>79.700299999999999</v>
       </c>
       <c r="Q10" s="34">
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R10" s="7">
-        <v>291.99400000000003</v>
+        <v>288.25150000000002</v>
       </c>
       <c r="S10" s="24">
         <f t="shared" si="0"/>
-        <v>283.74792963960653</v>
+        <v>284.23921728284932</v>
       </c>
       <c r="T10">
-        <f t="shared" si="1"/>
-        <v>8.2460703603935031</v>
+        <f t="shared" si="3"/>
+        <v>4.012282717150697</v>
       </c>
       <c r="U10">
-        <f t="shared" si="2"/>
-        <v>0.97071686102169785</v>
+        <f t="shared" si="4"/>
+        <v>0.71387489856796449</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25"/>
@@ -2313,22 +2618,22 @@
         <v>92.136600000000001</v>
       </c>
       <c r="Q11" s="34">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="R11" s="7">
-        <v>291.93689999999998</v>
+        <v>291.99400000000003</v>
       </c>
       <c r="S11" s="24">
         <f t="shared" si="0"/>
-        <v>285.16436486749222</v>
+        <v>286.59896475831698</v>
       </c>
       <c r="T11">
-        <f t="shared" si="1"/>
-        <v>6.7725351325077554</v>
+        <f t="shared" si="3"/>
+        <v>5.3950352416830469</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
-        <v>0.96711728392321772</v>
+        <f t="shared" si="4"/>
+        <v>0.68031646916885991</v>
       </c>
       <c r="W11" s="27" t="s">
         <v>5</v>
@@ -2392,22 +2697,22 @@
         <v>102.4306</v>
       </c>
       <c r="Q12" s="34">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="R12" s="7">
-        <v>291.85809999999998</v>
+        <v>291.93689999999998</v>
       </c>
       <c r="S12" s="24">
         <f t="shared" si="0"/>
-        <v>286.31902865926725</v>
+        <v>288.35018107338431</v>
       </c>
       <c r="T12">
-        <f t="shared" si="1"/>
-        <v>5.5390713407327326</v>
+        <f t="shared" si="3"/>
+        <v>3.5867189266156743</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
-        <v>0.96353105464613442</v>
+        <f t="shared" si="4"/>
+        <v>0.64833558253809442</v>
       </c>
       <c r="W12" s="27" t="s">
         <v>4</v>
@@ -2467,28 +2772,28 @@
         <v>110.6581</v>
       </c>
       <c r="Q13" s="34">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="R13" s="7">
-        <v>291.75209999999998</v>
+        <v>291.85809999999998</v>
       </c>
       <c r="S13" s="24">
         <f t="shared" si="0"/>
-        <v>287.26016626965634</v>
+        <v>289.62473022914895</v>
       </c>
       <c r="T13">
-        <f t="shared" si="1"/>
-        <v>4.4919337303436464</v>
+        <f t="shared" si="3"/>
+        <v>2.2333697708510272</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
-        <v>0.95995812369454037</v>
+        <f t="shared" si="4"/>
+        <v>0.61785808022336541</v>
       </c>
       <c r="W13" s="27" t="s">
         <v>9</v>
       </c>
       <c r="X13" s="27">
-        <v>0.18575280283275319</v>
+        <v>2.407482457740497</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.2">
@@ -2541,29 +2846,29 @@
         <v>117.2449</v>
       </c>
       <c r="Q14" s="34">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="R14" s="7">
-        <v>291.61669999999998</v>
+        <v>291.75209999999998</v>
       </c>
       <c r="S14" s="24">
         <f t="shared" si="0"/>
-        <v>288.02375081427164</v>
+        <v>290.51980048686238</v>
       </c>
       <c r="T14">
-        <f t="shared" si="1"/>
-        <v>3.5929491857283438</v>
+        <f t="shared" si="3"/>
+        <v>1.2322995131376047</v>
       </c>
       <c r="U14">
-        <f t="shared" si="2"/>
-        <v>0.95639844175606659</v>
+        <f t="shared" si="4"/>
+        <v>0.58881328987503501</v>
       </c>
       <c r="V14" s="11"/>
       <c r="W14" s="27" t="s">
         <v>10</v>
       </c>
       <c r="X14" s="27">
-        <v>15.18525234456194</v>
+        <v>8.8723113918844163</v>
       </c>
       <c r="Y14" s="11"/>
     </row>
@@ -2617,29 +2922,29 @@
         <v>122.6557</v>
       </c>
       <c r="Q15" s="34">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="R15" s="7">
-        <v>291.44920000000002</v>
+        <v>291.61669999999998</v>
       </c>
       <c r="S15" s="24">
         <f t="shared" si="0"/>
-        <v>288.63734915917053</v>
+        <v>291.109174733131</v>
       </c>
       <c r="T15">
-        <f t="shared" si="1"/>
-        <v>2.8118508408294929</v>
+        <f t="shared" si="3"/>
+        <v>0.50752526686898136</v>
       </c>
       <c r="U15">
-        <f t="shared" si="2"/>
-        <v>0.95285195970120262</v>
+        <f t="shared" si="4"/>
+        <v>0.56113386136849452</v>
       </c>
       <c r="V15" s="11"/>
       <c r="W15" s="27" t="s">
         <v>0</v>
       </c>
       <c r="X15" s="27">
-        <v>7.562407723183312E-2</v>
+        <v>0.12697683971386639</v>
       </c>
       <c r="Y15" s="11"/>
     </row>
@@ -2693,29 +2998,29 @@
         <v>127.2582</v>
       </c>
       <c r="Q16" s="34">
-        <v>0.28000000000000003</v>
+        <v>0.26</v>
       </c>
       <c r="R16" s="7">
-        <v>291.24740000000003</v>
+        <v>291.44920000000002</v>
       </c>
       <c r="S16" s="24">
         <f t="shared" si="0"/>
-        <v>289.12257107575414</v>
+        <v>291.45018865093266</v>
       </c>
       <c r="T16">
-        <f t="shared" si="1"/>
-        <v>2.1248289242458895</v>
+        <f t="shared" si="3"/>
+        <v>9.8865093264066672E-4</v>
       </c>
       <c r="U16">
-        <f t="shared" si="2"/>
-        <v>0.9493186285826184</v>
+        <f t="shared" si="4"/>
+        <v>0.53475561063022625</v>
       </c>
       <c r="V16" s="11"/>
       <c r="W16" s="27" t="s">
         <v>11</v>
       </c>
       <c r="X16" s="27">
-        <v>-0.12428749909353851</v>
+        <v>14.430114566415607</v>
       </c>
       <c r="Y16" s="11"/>
     </row>
@@ -2769,29 +3074,29 @@
         <v>131.32300000000001</v>
       </c>
       <c r="Q17" s="34">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R17" s="7">
-        <v>291.01069999999999</v>
+        <v>291.24740000000003</v>
       </c>
       <c r="S17" s="24">
         <f t="shared" si="0"/>
-        <v>289.49668355192915</v>
+        <v>291.58823686845068</v>
       </c>
       <c r="T17">
-        <f t="shared" si="1"/>
-        <v>1.5140164480708336</v>
+        <f t="shared" si="3"/>
+        <v>0.34083686845065131</v>
       </c>
       <c r="U17">
-        <f t="shared" si="2"/>
-        <v>0.9457983996344882</v>
+        <f t="shared" si="4"/>
+        <v>0.50961737080542158</v>
       </c>
       <c r="V17" s="11"/>
       <c r="W17" s="27" t="s">
         <v>12</v>
       </c>
       <c r="X17" s="27">
-        <v>-0.79425713330758629</v>
+        <v>6.3844803589954573</v>
       </c>
       <c r="Y17" s="11"/>
     </row>
@@ -2845,29 +3150,29 @@
         <v>135.0538</v>
       </c>
       <c r="Q18" s="34">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="R18" s="7">
-        <v>290.73439999999999</v>
+        <v>291.01069999999999</v>
       </c>
       <c r="S18" s="24">
         <f t="shared" si="0"/>
-        <v>289.77371075464004</v>
+        <v>291.55980814685705</v>
       </c>
       <c r="T18">
-        <f t="shared" si="1"/>
-        <v>0.96068924535995848</v>
+        <f t="shared" si="3"/>
+        <v>0.54910814685706555</v>
       </c>
       <c r="U18">
-        <f t="shared" si="2"/>
-        <v>0.94229122427181833</v>
+        <f t="shared" si="4"/>
+        <v>0.48566085042203561</v>
       </c>
       <c r="V18" s="11"/>
       <c r="W18" s="27" t="s">
         <v>14</v>
       </c>
       <c r="X18" s="27">
-        <v>0.11433082675050535</v>
+        <v>-12.424444541309043</v>
       </c>
       <c r="Y18" s="11"/>
     </row>
@@ -2921,29 +3226,29 @@
         <v>138.58600000000001</v>
       </c>
       <c r="Q19" s="34">
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="R19" s="7">
-        <v>290.4187</v>
+        <v>290.73439999999999</v>
       </c>
       <c r="S19" s="24">
         <f t="shared" si="0"/>
-        <v>289.96520499937429</v>
+        <v>291.39459814759186</v>
       </c>
       <c r="T19">
-        <f t="shared" si="1"/>
-        <v>0.45349500062570769</v>
+        <f t="shared" si="3"/>
+        <v>0.66019814759187057</v>
       </c>
       <c r="U19">
-        <f t="shared" si="2"/>
-        <v>0.9387970540897761</v>
+        <f t="shared" si="4"/>
+        <v>0.46283049822238431</v>
       </c>
       <c r="V19" s="11"/>
       <c r="W19" s="27" t="s">
         <v>1</v>
       </c>
       <c r="X19" s="27">
-        <v>4.6399136524414644</v>
+        <v>5.789545005974281</v>
       </c>
       <c r="Y19" s="11"/>
     </row>
@@ -2997,22 +3302,22 @@
         <v>141.98939999999999</v>
       </c>
       <c r="Q20" s="34">
-        <v>0.36</v>
+        <v>0.34</v>
       </c>
       <c r="R20" s="7">
-        <v>290.07139999999998</v>
+        <v>290.4187</v>
       </c>
       <c r="S20" s="24">
         <f t="shared" si="0"/>
-        <v>290.08080044079816</v>
+        <v>291.11702174845163</v>
       </c>
       <c r="T20">
-        <f t="shared" si="1"/>
-        <v>9.4004407981742588E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.69832174845163308</v>
       </c>
       <c r="U20">
-        <f t="shared" si="2"/>
-        <v>0.93531584086302166</v>
+        <f t="shared" si="4"/>
+        <v>0.4410733743488523</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
@@ -3065,22 +3370,22 @@
         <v>145.2585</v>
       </c>
       <c r="Q21" s="34">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="R21" s="7">
-        <v>289.6884</v>
+        <v>290.07139999999998</v>
       </c>
       <c r="S21" s="24">
         <f t="shared" si="0"/>
-        <v>290.12861923806435</v>
+        <v>290.74732181536058</v>
       </c>
       <c r="T21">
-        <f t="shared" si="1"/>
-        <v>0.44021923806434415</v>
+        <f t="shared" si="3"/>
+        <v>0.6759218153605957</v>
       </c>
       <c r="U21">
-        <f t="shared" si="2"/>
-        <v>0.93184753654504304</v>
+        <f t="shared" si="4"/>
+        <v>0.42033902758501018</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
@@ -3133,22 +3438,22 @@
         <v>148.32929999999999</v>
       </c>
       <c r="Q22" s="34">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="R22" s="7">
-        <v>289.27229999999997</v>
+        <v>289.6884</v>
       </c>
       <c r="S22" s="24">
         <f t="shared" si="0"/>
-        <v>290.11557510444641</v>
+        <v>290.30239917134031</v>
       </c>
       <c r="T22">
-        <f t="shared" si="1"/>
-        <v>0.84327510444643394</v>
+        <f t="shared" si="3"/>
+        <v>0.61399917134031057</v>
       </c>
       <c r="U22">
-        <f t="shared" si="2"/>
-        <v>0.92839209326749217</v>
+        <f t="shared" si="4"/>
+        <v>0.40057937836748425</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
@@ -3201,22 +3506,22 @@
         <v>151.13509999999999</v>
       </c>
       <c r="Q23" s="34">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
       <c r="R23" s="7">
-        <v>288.8331</v>
+        <v>289.27229999999997</v>
       </c>
       <c r="S23" s="24">
         <f t="shared" si="0"/>
-        <v>290.04760394262308</v>
+        <v>289.79644524143504</v>
       </c>
       <c r="T23">
-        <f t="shared" si="1"/>
-        <v>1.2145039426230824</v>
+        <f t="shared" si="3"/>
+        <v>0.52414524143506469</v>
       </c>
       <c r="U23">
-        <f t="shared" si="2"/>
-        <v>0.92494946333952488</v>
+        <f t="shared" si="4"/>
+        <v>0.38174860729730264</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -3269,22 +3574,22 @@
         <v>153.69229999999999</v>
       </c>
       <c r="Q24" s="34">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="R24" s="7">
-        <v>288.36279999999999</v>
+        <v>288.8331</v>
       </c>
       <c r="S24" s="24">
         <f t="shared" si="0"/>
-        <v>289.92984168041551</v>
+        <v>289.24143204036159</v>
       </c>
       <c r="T24">
-        <f t="shared" si="1"/>
-        <v>1.5670416804155138</v>
+        <f t="shared" si="3"/>
+        <v>0.40833204036158577</v>
       </c>
       <c r="U24">
-        <f t="shared" si="2"/>
-        <v>0.92151959924714244</v>
+        <f t="shared" si="4"/>
+        <v>0.36380304889219317</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -3337,22 +3642,22 @@
         <v>156.1122</v>
       </c>
       <c r="Q25" s="34">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="R25" s="7">
-        <v>287.88170000000002</v>
+        <v>288.36279999999999</v>
       </c>
       <c r="S25" s="24">
         <f t="shared" si="0"/>
-        <v>289.76676322021029</v>
+        <v>288.64749706072621</v>
       </c>
       <c r="T25">
-        <f t="shared" si="1"/>
-        <v>1.8850632202102702</v>
+        <f t="shared" si="3"/>
+        <v>0.28469706072621648</v>
       </c>
       <c r="U25">
-        <f t="shared" si="2"/>
-        <v>0.91810245365253584</v>
+        <f t="shared" si="4"/>
+        <v>0.34670109033346203</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
@@ -3399,22 +3704,22 @@
         <v>158.5137</v>
       </c>
       <c r="Q26" s="34">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="R26" s="7">
-        <v>287.36669999999998</v>
+        <v>287.88170000000002</v>
       </c>
       <c r="S26" s="24">
         <f t="shared" si="0"/>
-        <v>289.56229230960747</v>
+        <v>288.02324941620788</v>
       </c>
       <c r="T26">
-        <f t="shared" si="1"/>
-        <v>2.1955923096074912</v>
+        <f t="shared" si="3"/>
+        <v>0.14154941620785166</v>
       </c>
       <c r="U26">
-        <f t="shared" si="2"/>
-        <v>0.91469797939343223</v>
+        <f t="shared" si="4"/>
+        <v>0.33040307497266508</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
@@ -3461,22 +3766,22 @@
         <v>160.90889999999999</v>
       </c>
       <c r="Q27" s="34">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="R27" s="7">
-        <v>286.8544</v>
+        <v>287.36669999999998</v>
       </c>
       <c r="S27" s="24">
         <f t="shared" si="0"/>
-        <v>289.31988936566091</v>
+        <v>287.37601608634117</v>
       </c>
       <c r="T27">
-        <f t="shared" si="1"/>
-        <v>2.4654893656609147</v>
+        <f t="shared" si="3"/>
+        <v>9.3160863411867467E-3</v>
       </c>
       <c r="U27">
-        <f t="shared" si="2"/>
-        <v>0.9113061294824446</v>
+        <f t="shared" si="4"/>
+        <v>0.31487121037431676</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -3523,22 +3828,22 @@
         <v>163.14609999999999</v>
       </c>
       <c r="Q28" s="34">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="R28" s="7">
-        <v>284.1146</v>
+        <v>286.8544</v>
       </c>
       <c r="S28" s="24">
         <f t="shared" si="0"/>
-        <v>287.63550067687703</v>
+        <v>286.71204197286318</v>
       </c>
       <c r="T28">
-        <f t="shared" si="1"/>
-        <v>3.5209006768770337</v>
+        <f t="shared" si="3"/>
+        <v>0.14235802713682233</v>
       </c>
       <c r="U28">
-        <f t="shared" si="2"/>
-        <v>0.89453461275115909</v>
+        <f t="shared" si="4"/>
+        <v>0.30006948068140599</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -3585,22 +3890,22 @@
         <v>164.9776</v>
       </c>
       <c r="Q29" s="34">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="R29" s="7">
-        <v>281.33589999999998</v>
+        <v>284.1146</v>
       </c>
       <c r="S29" s="24">
         <f t="shared" si="0"/>
-        <v>285.35004588911443</v>
+        <v>283.30235363563509</v>
       </c>
       <c r="T29">
-        <f t="shared" si="1"/>
-        <v>4.0141458891144453</v>
+        <f t="shared" si="3"/>
+        <v>0.81224636436490982</v>
       </c>
       <c r="U29">
-        <f t="shared" si="2"/>
-        <v>0.87807175604570653</v>
+        <f t="shared" si="4"/>
+        <v>0.23586646163265487</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
@@ -3647,22 +3952,22 @@
         <v>166.23779999999999</v>
       </c>
       <c r="Q30" s="34">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="R30" s="7">
-        <v>278.65370000000001</v>
+        <v>281.33589999999998</v>
       </c>
       <c r="S30" s="24">
         <f t="shared" si="0"/>
-        <v>282.63882253169038</v>
+        <v>280.01094271643501</v>
       </c>
       <c r="T30">
-        <f t="shared" si="1"/>
-        <v>3.9851225316903651</v>
+        <f t="shared" si="3"/>
+        <v>1.3249572835649701</v>
       </c>
       <c r="U30">
-        <f t="shared" si="2"/>
-        <v>0.86191187884159581</v>
+        <f t="shared" si="4"/>
+        <v>0.18540035326743576</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
@@ -3705,22 +4010,22 @@
         <v>166.98349999999999</v>
       </c>
       <c r="Q31" s="34">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="R31" s="7">
-        <v>276.11020000000002</v>
+        <v>278.65370000000001</v>
       </c>
       <c r="S31" s="24">
         <f t="shared" si="0"/>
-        <v>279.6168804963234</v>
+        <v>277.02751904406716</v>
       </c>
       <c r="T31">
-        <f t="shared" si="1"/>
-        <v>3.5066804963233835</v>
+        <f t="shared" si="3"/>
+        <v>1.6261809559328526</v>
       </c>
       <c r="U31">
-        <f t="shared" si="2"/>
-        <v>0.84604940515770299</v>
+        <f t="shared" si="4"/>
+        <v>0.14573199917343019</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
@@ -3763,22 +4068,22 @@
         <v>167.47880000000001</v>
       </c>
       <c r="Q32" s="34">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="R32" s="7">
-        <v>273.72609999999997</v>
+        <v>276.11020000000002</v>
       </c>
       <c r="S32" s="24">
         <f t="shared" si="0"/>
-        <v>276.36391188030075</v>
+        <v>274.41755069974454</v>
       </c>
       <c r="T32">
-        <f t="shared" si="1"/>
-        <v>2.6378118803007737</v>
+        <f t="shared" si="3"/>
+        <v>1.6926493002554821</v>
       </c>
       <c r="U32">
-        <f t="shared" si="2"/>
-        <v>0.83047886163227402</v>
+        <f t="shared" si="4"/>
+        <v>0.11455110634255158</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
@@ -3821,22 +4126,22 @@
         <v>168.035</v>
       </c>
       <c r="Q33" s="34">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="R33" s="7">
-        <v>271.4889</v>
+        <v>273.72609999999997</v>
       </c>
       <c r="S33" s="24">
         <f t="shared" si="0"/>
-        <v>272.93742135852062</v>
+        <v>272.18489093075505</v>
       </c>
       <c r="T33">
-        <f t="shared" si="1"/>
-        <v>1.4485213585206225</v>
+        <f t="shared" si="3"/>
+        <v>1.5412090692449283</v>
       </c>
       <c r="U33">
-        <f t="shared" si="2"/>
-        <v>0.81519487563433624</v>
+        <f t="shared" si="4"/>
+        <v>9.0041693236408676E-2</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
@@ -3879,22 +4184,22 @@
         <v>168.8511</v>
       </c>
       <c r="Q34" s="34">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="R34" s="7">
-        <v>269.40100000000001</v>
+        <v>271.4889</v>
       </c>
       <c r="S34" s="24">
         <f t="shared" si="0"/>
-        <v>269.38025021244636</v>
+        <v>270.30391816760095</v>
       </c>
       <c r="T34">
-        <f t="shared" si="1"/>
-        <v>2.0749787553654642E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.1849818323990462</v>
       </c>
       <c r="U34">
-        <f t="shared" si="2"/>
-        <v>0.80019217340986615</v>
+        <f t="shared" si="4"/>
+        <v>7.0776326652271501E-2</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
@@ -3937,22 +4242,22 @@
         <v>169.93289999999999</v>
       </c>
       <c r="Q35" s="34">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="R35" s="7">
-        <v>267.4479</v>
+        <v>269.40100000000001</v>
       </c>
       <c r="S35" s="24">
-        <f t="shared" ref="S35:S62" si="3">SQRT(3)*(U35*$X$14*(Q35^$X$15)*EXP($X$16/$Q$1)+(1-U35)*$X$17*EXP($X$18/$Q$1))*(SQRT(3)*$AA$11)^$X$19</f>
-        <v>265.72513982113162</v>
+        <f t="shared" ref="S35:S63" si="5">SQRT(3)*(U35*$X$14*(Q35^$X$15)*EXP($X$16/$Q$1)+(1-U35)*$X$17*EXP($X$18/$Q$1))*(SQRT(3)*$AA$11)^$X$19</f>
+        <v>268.73652053929567</v>
       </c>
       <c r="T35">
-        <f t="shared" si="1"/>
-        <v>1.7227601788683842</v>
+        <f t="shared" si="3"/>
+        <v>0.66447946070434227</v>
       </c>
       <c r="U35">
-        <f t="shared" si="2"/>
-        <v>0.78546557826207641</v>
+        <f t="shared" si="4"/>
+        <v>5.5632987723108651E-2</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
@@ -3995,22 +4300,22 @@
         <v>171.14709999999999</v>
       </c>
       <c r="Q36" s="34">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="R36" s="7">
-        <v>265.61750000000001</v>
+        <v>267.4479</v>
       </c>
       <c r="S36" s="24">
+        <f t="shared" si="5"/>
+        <v>267.44110282690588</v>
+      </c>
+      <c r="T36">
         <f t="shared" si="3"/>
-        <v>261.99763605408333</v>
-      </c>
-      <c r="T36">
-        <f t="shared" si="1"/>
-        <v>3.619863945916677</v>
+        <v>6.7971730941280839E-3</v>
       </c>
       <c r="U36">
-        <f t="shared" si="2"/>
-        <v>0.77101000876519088</v>
+        <f t="shared" si="4"/>
+        <v>4.3729725310634293E-2</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
@@ -4053,22 +4358,22 @@
         <v>172.34899999999999</v>
       </c>
       <c r="Q37" s="34">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="R37" s="7">
-        <v>263.90519999999998</v>
+        <v>265.61750000000001</v>
       </c>
       <c r="S37" s="24">
+        <f t="shared" si="5"/>
+        <v>266.37724352284613</v>
+      </c>
+      <c r="T37">
         <f t="shared" si="3"/>
-        <v>258.21801246650381</v>
-      </c>
-      <c r="T37">
-        <f t="shared" si="1"/>
-        <v>5.6871875334961715</v>
+        <v>0.75974352284612223</v>
       </c>
       <c r="U37">
-        <f t="shared" si="2"/>
-        <v>0.75682047701109434</v>
+        <f t="shared" si="4"/>
+        <v>3.4373290991689981E-2</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
@@ -4111,22 +4416,22 @@
         <v>173.4718</v>
       </c>
       <c r="Q38" s="34">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="R38" s="7">
-        <v>262.2679</v>
+        <v>263.90519999999998</v>
       </c>
       <c r="S38" s="24">
+        <f t="shared" si="5"/>
+        <v>265.50793732816174</v>
+      </c>
+      <c r="T38">
         <f t="shared" si="3"/>
-        <v>254.40258678226894</v>
-      </c>
-      <c r="T38">
-        <f t="shared" si="1"/>
-        <v>7.8653132177310567</v>
+        <v>1.6027373281617656</v>
       </c>
       <c r="U38">
-        <f t="shared" si="2"/>
-        <v>0.7428920868882497</v>
+        <f t="shared" si="4"/>
+        <v>2.7018764129123615E-2</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
@@ -4169,22 +4474,22 @@
         <v>174.524</v>
       </c>
       <c r="Q39" s="34">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="R39" s="7">
-        <v>260.73930000000001</v>
+        <v>262.2679</v>
       </c>
       <c r="S39" s="24">
+        <f t="shared" si="5"/>
+        <v>264.80049502256753</v>
+      </c>
+      <c r="T39">
         <f t="shared" si="3"/>
-        <v>250.56464788977149</v>
-      </c>
-      <c r="T39">
-        <f t="shared" si="1"/>
-        <v>10.174652110228521</v>
+        <v>2.5325950225675342</v>
       </c>
       <c r="U39">
-        <f t="shared" si="2"/>
-        <v>0.72922003239229027</v>
+        <f t="shared" si="4"/>
+        <v>2.1237815583084661E-2</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
@@ -4227,22 +4532,22 @@
         <v>175.5437</v>
       </c>
       <c r="Q40" s="34">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="R40" s="7">
-        <v>259.27969999999999</v>
+        <v>260.73930000000001</v>
       </c>
       <c r="S40" s="24">
+        <f t="shared" si="5"/>
+        <v>264.22670905139574</v>
+      </c>
+      <c r="T40">
         <f t="shared" si="3"/>
-        <v>246.71512466330813</v>
-      </c>
-      <c r="T40">
-        <f t="shared" si="1"/>
-        <v>12.56457533669186</v>
+        <v>3.4874090513957299</v>
       </c>
       <c r="U40">
-        <f t="shared" si="2"/>
-        <v>0.71579959596770293</v>
+        <f t="shared" si="4"/>
+        <v>1.6693761734828245E-2</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
@@ -4285,22 +4590,22 @@
         <v>176.54849999999999</v>
       </c>
       <c r="Q41" s="34">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="R41" s="7">
-        <v>257.91379999999998</v>
+        <v>259.27969999999999</v>
       </c>
       <c r="S41" s="24">
+        <f t="shared" si="5"/>
+        <v>263.76263459311076</v>
+      </c>
+      <c r="T41">
         <f t="shared" si="3"/>
-        <v>242.86307884621806</v>
-      </c>
-      <c r="T41">
-        <f t="shared" si="1"/>
-        <v>15.050721153781922</v>
+        <v>4.4829345931107696</v>
       </c>
       <c r="U41">
-        <f t="shared" si="2"/>
-        <v>0.70262614688003178</v>
+        <f t="shared" si="4"/>
+        <v>1.3121955964302563E-2</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
@@ -4339,22 +4644,22 @@
         <v>177.5163</v>
       </c>
       <c r="Q42" s="34">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="R42" s="7">
-        <v>256.59030000000001</v>
+        <v>257.91379999999998</v>
       </c>
       <c r="S42" s="24">
+        <f t="shared" si="5"/>
+        <v>263.38818760962107</v>
+      </c>
+      <c r="T42">
         <f t="shared" si="3"/>
-        <v>239.01607510130512</v>
-      </c>
-      <c r="T42">
-        <f t="shared" si="1"/>
-        <v>17.574224898694894</v>
+        <v>5.4743876096210897</v>
       </c>
       <c r="U42">
-        <f t="shared" si="2"/>
-        <v>0.68969513961803774</v>
+        <f t="shared" si="4"/>
+        <v>1.0314375577187262E-2</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
@@ -4393,22 +4698,22 @@
         <v>178.41079999999999</v>
       </c>
       <c r="Q43" s="34">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="R43" s="7">
-        <v>255.33779999999999</v>
+        <v>256.59030000000001</v>
       </c>
       <c r="S43" s="24">
+        <f t="shared" si="5"/>
+        <v>263.08667477074783</v>
+      </c>
+      <c r="T43">
         <f t="shared" si="3"/>
-        <v>235.18046345628127</v>
-      </c>
-      <c r="T43">
-        <f t="shared" si="1"/>
-        <v>20.157336543718714</v>
+        <v>6.4963747707478205</v>
       </c>
       <c r="U43">
-        <f t="shared" si="2"/>
-        <v>0.67700211232526675</v>
+        <f t="shared" si="4"/>
+        <v>8.107506520879524E-3</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
@@ -4447,22 +4752,22 @@
         <v>179.196</v>
       </c>
       <c r="Q44" s="34">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="R44" s="7">
-        <v>254.14789999999999</v>
+        <v>255.33779999999999</v>
       </c>
       <c r="S44" s="24">
+        <f t="shared" si="5"/>
+        <v>262.84431900555984</v>
+      </c>
+      <c r="T44">
         <f t="shared" si="3"/>
-        <v>231.36159807405718</v>
-      </c>
-      <c r="T44">
-        <f t="shared" si="1"/>
-        <v>22.786301925942809</v>
+        <v>7.5065190055598521</v>
       </c>
       <c r="U44">
-        <f t="shared" si="2"/>
-        <v>0.66454268526048088</v>
+        <f t="shared" si="4"/>
+        <v>6.3728202928236858E-3</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
@@ -4501,22 +4806,22 @@
         <v>179.84729999999999</v>
       </c>
       <c r="Q45" s="34">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="R45" s="7">
-        <v>253.0121</v>
+        <v>254.14789999999999</v>
       </c>
       <c r="S45" s="24">
+        <f t="shared" si="5"/>
+        <v>262.64981415520498</v>
+      </c>
+      <c r="T45">
         <f t="shared" si="3"/>
-        <v>227.56400895036279</v>
-      </c>
-      <c r="T45">
-        <f t="shared" si="1"/>
-        <v>25.448091049637213</v>
+        <v>8.5019141552049859</v>
       </c>
       <c r="U45">
-        <f t="shared" si="2"/>
-        <v>0.65231255928642506</v>
+        <f t="shared" si="4"/>
+        <v>5.0092884143890367E-3</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
@@ -4551,22 +4856,22 @@
         <v>180.3603</v>
       </c>
       <c r="Q46" s="34">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R46" s="7">
-        <v>251.92359999999999</v>
+        <v>253.0121</v>
       </c>
       <c r="S46" s="24">
+        <f t="shared" si="5"/>
+        <v>262.49392438186777</v>
+      </c>
+      <c r="T46">
         <f t="shared" si="3"/>
-        <v>223.79153827774786</v>
-      </c>
-      <c r="T46">
-        <f t="shared" si="1"/>
-        <v>28.132061722252132</v>
+        <v>9.4818243818677672</v>
       </c>
       <c r="U46">
-        <f t="shared" si="2"/>
-        <v>0.64030751438640532</v>
+        <f t="shared" si="4"/>
+        <v>3.9374985117325489E-3</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
@@ -4597,22 +4902,22 @@
       <c r="O47" s="7"/>
       <c r="P47" s="7"/>
       <c r="Q47" s="34">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="R47" s="7">
-        <v>250.87530000000001</v>
+        <v>251.92359999999999</v>
       </c>
       <c r="S47" s="24">
+        <f t="shared" si="5"/>
+        <v>262.36913367909739</v>
+      </c>
+      <c r="T47">
         <f t="shared" si="3"/>
-        <v>220.04744991920185</v>
-      </c>
-      <c r="T47">
-        <f t="shared" si="1"/>
-        <v>30.827850080798157</v>
+        <v>10.445533679097394</v>
       </c>
       <c r="U47">
-        <f t="shared" si="2"/>
-        <v>0.62852340820816821</v>
+        <f t="shared" si="4"/>
+        <v>3.0950293229995577E-3</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
@@ -4643,22 +4948,22 @@
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
       <c r="Q48" s="34">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="R48" s="7">
-        <v>249.8673</v>
+        <v>250.87530000000001</v>
       </c>
       <c r="S48" s="24">
+        <f t="shared" si="5"/>
+        <v>262.26934506321521</v>
+      </c>
+      <c r="T48">
         <f t="shared" si="3"/>
-        <v>216.33451815886355</v>
-      </c>
-      <c r="T48">
-        <f t="shared" si="1"/>
-        <v>33.532781841136455</v>
+        <v>11.394045063215202</v>
       </c>
       <c r="U48">
-        <f t="shared" si="2"/>
-        <v>0.61695617463457808</v>
+        <f t="shared" si="4"/>
+        <v>2.4328152713414325E-3</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
@@ -4689,22 +4994,22 @@
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="34">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="R49" s="7">
-        <v>248.8998</v>
+        <v>249.8673</v>
       </c>
       <c r="S49" s="24">
+        <f t="shared" si="5"/>
+        <v>262.18962600096256</v>
+      </c>
+      <c r="T49">
         <f t="shared" si="3"/>
-        <v>212.65510029887395</v>
-      </c>
-      <c r="T49">
-        <f t="shared" si="1"/>
-        <v>36.244699701126052</v>
+        <v>12.322326000962562</v>
       </c>
       <c r="U49">
-        <f t="shared" si="2"/>
-        <v>0.60560182238059912</v>
+        <f t="shared" si="4"/>
+        <v>1.9122888757435298E-3</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
@@ -4723,22 +5028,22 @@
       <c r="O50" s="7"/>
       <c r="P50" s="7"/>
       <c r="Q50" s="34">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="R50" s="7">
-        <v>247.96260000000001</v>
+        <v>248.8998</v>
       </c>
       <c r="S50" s="24">
+        <f t="shared" si="5"/>
+        <v>262.1259952397748</v>
+      </c>
+      <c r="T50">
         <f t="shared" si="3"/>
-        <v>209.01119653118462</v>
-      </c>
-      <c r="T50">
-        <f t="shared" si="1"/>
-        <v>38.951403468815386</v>
+        <v>13.226195239774796</v>
       </c>
       <c r="U50">
-        <f t="shared" si="2"/>
-        <v>0.59445643361609968</v>
+        <f t="shared" si="4"/>
+        <v>1.5031345730891024E-3</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
@@ -4757,22 +5062,22 @@
       <c r="O51" s="7"/>
       <c r="P51" s="7"/>
       <c r="Q51" s="34">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="R51" s="7">
-        <v>247.05719999999999</v>
+        <v>247.96260000000001</v>
       </c>
       <c r="S51" s="24">
+        <f t="shared" si="5"/>
+        <v>262.07524577376159</v>
+      </c>
+      <c r="T51">
         <f t="shared" si="3"/>
-        <v>205.40449968808477</v>
-      </c>
-      <c r="T51">
-        <f t="shared" si="1"/>
-        <v>41.652700311915225</v>
+        <v>14.112645773761585</v>
       </c>
       <c r="U51">
-        <f t="shared" si="2"/>
-        <v>0.58351616261399974</v>
+        <f t="shared" si="4"/>
+        <v>1.1815231335993955E-3</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
@@ -4791,22 +5096,22 @@
       <c r="O52" s="7"/>
       <c r="P52" s="7"/>
       <c r="Q52" s="34">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="R52" s="7">
-        <v>246.18350000000001</v>
+        <v>247.05719999999999</v>
       </c>
       <c r="S52" s="24">
+        <f t="shared" si="5"/>
+        <v>262.03479878214819</v>
+      </c>
+      <c r="T52">
         <f t="shared" si="3"/>
-        <v>201.83643687036991</v>
-      </c>
-      <c r="T52">
-        <f t="shared" si="1"/>
-        <v>44.347063129630101</v>
+        <v>14.977598782148192</v>
       </c>
       <c r="U52">
-        <f t="shared" si="2"/>
-        <v>0.57277723442330031</v>
+        <f t="shared" si="4"/>
+        <v>9.287238416462012E-4</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
@@ -4825,22 +5130,22 @@
       <c r="O53" s="7"/>
       <c r="P53" s="7"/>
       <c r="Q53" s="34">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="R53" s="7">
-        <v>245.3408</v>
+        <v>246.18350000000001</v>
       </c>
       <c r="S53" s="24">
+        <f t="shared" si="5"/>
+        <v>262.00258376184746</v>
+      </c>
+      <c r="T53">
         <f t="shared" si="3"/>
-        <v>198.30820450328952</v>
-      </c>
-      <c r="T53">
-        <f t="shared" si="1"/>
-        <v>47.032595496710485</v>
+        <v>15.819083761847452</v>
       </c>
       <c r="U53">
-        <f t="shared" si="2"/>
-        <v>0.56223594356653239</v>
+        <f t="shared" si="4"/>
+        <v>7.3001361506521702E-4</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
@@ -4855,22 +5160,22 @@
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
       <c r="Q54" s="34">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="R54" s="7">
-        <v>244.52930000000001</v>
+        <v>245.3408</v>
       </c>
       <c r="S54" s="24">
+        <f t="shared" si="5"/>
+        <v>261.97694058782798</v>
+      </c>
+      <c r="T54">
         <f t="shared" si="3"/>
-        <v>194.82079803367273</v>
-      </c>
-      <c r="T54">
-        <f t="shared" si="1"/>
-        <v>49.708501966327276</v>
+        <v>16.636140587827981</v>
       </c>
       <c r="U54">
-        <f t="shared" si="2"/>
-        <v>0.55188865276117871</v>
+        <f t="shared" si="4"/>
+        <v>5.7381952985719039E-4</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
@@ -4885,22 +5190,22 @@
       <c r="O55" s="7"/>
       <c r="P55" s="7"/>
       <c r="Q55" s="34">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="R55" s="7">
-        <v>243.74959999999999</v>
+        <v>244.52930000000001</v>
       </c>
       <c r="S55" s="24">
+        <f t="shared" si="5"/>
+        <v>261.95653978332768</v>
+      </c>
+      <c r="T55">
         <f t="shared" si="3"/>
-        <v>191.37503722634349</v>
-      </c>
-      <c r="T55">
-        <f t="shared" si="1"/>
-        <v>52.374562773656493</v>
+        <v>17.427239783327678</v>
       </c>
       <c r="U55">
-        <f t="shared" si="2"/>
-        <v>0.54173179166462559</v>
+        <f t="shared" si="4"/>
+        <v>4.5104481074111368E-4</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
@@ -4915,22 +5220,22 @@
       <c r="O56" s="7"/>
       <c r="P56" s="7"/>
       <c r="Q56" s="34">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="R56" s="7">
-        <v>242.9897</v>
+        <v>243.74959999999999</v>
       </c>
       <c r="S56" s="24">
+        <f t="shared" si="5"/>
+        <v>261.94031781556856</v>
+      </c>
+      <c r="T56">
         <f t="shared" si="3"/>
-        <v>187.97158782251188</v>
-      </c>
-      <c r="T56">
-        <f t="shared" si="1"/>
-        <v>55.018112177488121</v>
+        <v>18.190717815568576</v>
       </c>
       <c r="U56">
-        <f t="shared" si="2"/>
-        <v>0.53176185564221279</v>
+        <f t="shared" si="4"/>
+        <v>3.545390331122379E-4</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
@@ -4945,22 +5250,22 @@
       <c r="O57" s="7"/>
       <c r="P57" s="7"/>
       <c r="Q57" s="34">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="R57" s="7">
-        <v>242.24029999999999</v>
+        <v>242.9897</v>
       </c>
       <c r="S57" s="24">
+        <f t="shared" si="5"/>
+        <v>261.92742472469661</v>
+      </c>
+      <c r="T57">
         <f t="shared" si="3"/>
-        <v>184.61098017188354</v>
-      </c>
-      <c r="T57">
-        <f t="shared" si="1"/>
-        <v>57.629319828116451</v>
+        <v>18.937724724696608</v>
       </c>
       <c r="U57">
-        <f t="shared" si="2"/>
-        <v>0.52197540455795666</v>
+        <f t="shared" si="4"/>
+        <v>2.7868168085921577E-4</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
@@ -4975,22 +5280,22 @@
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
       <c r="Q58" s="34">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="R58" s="7">
-        <v>241.52199999999999</v>
+        <v>242.24029999999999</v>
       </c>
       <c r="S58" s="24">
+        <f t="shared" si="5"/>
+        <v>261.91718183222912</v>
+      </c>
+      <c r="T58">
         <f t="shared" si="3"/>
-        <v>181.29362533265171</v>
-      </c>
-      <c r="T58">
-        <f t="shared" si="1"/>
-        <v>60.228374667348277</v>
+        <v>19.676881832229128</v>
       </c>
       <c r="U58">
-        <f t="shared" si="2"/>
-        <v>0.51236906158752682</v>
+        <f t="shared" si="4"/>
+        <v>2.1905480636297538E-4</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
@@ -5005,22 +5310,22 @@
       <c r="O59" s="7"/>
       <c r="P59" s="7"/>
       <c r="Q59" s="34">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="R59" s="7">
-        <v>240.83629999999999</v>
+        <v>241.52199999999999</v>
       </c>
       <c r="S59" s="24">
+        <f t="shared" si="5"/>
+        <v>261.90904765716965</v>
+      </c>
+      <c r="T59">
         <f t="shared" si="3"/>
-        <v>178.01982904122713</v>
-      </c>
-      <c r="T59">
-        <f t="shared" si="1"/>
-        <v>62.816470958772868</v>
+        <v>20.38704765716966</v>
       </c>
       <c r="U59">
-        <f t="shared" si="2"/>
-        <v>0.50293951205307064</v>
+        <f t="shared" si="4"/>
+        <v>1.7218572832909557E-4</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.2">
@@ -5035,22 +5340,22 @@
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="34">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="R60" s="7">
-        <v>240.14940000000001</v>
+        <v>240.83629999999999</v>
       </c>
       <c r="S60" s="24">
+        <f t="shared" si="5"/>
+        <v>261.90259049492767</v>
+      </c>
+      <c r="T60">
         <f t="shared" si="3"/>
-        <v>174.78980388054222</v>
-      </c>
-      <c r="T60">
-        <f t="shared" si="1"/>
-        <v>65.359596119457791</v>
+        <v>21.066290494927671</v>
       </c>
       <c r="U60">
-        <f t="shared" si="2"/>
-        <v>0.49368350227947994</v>
+        <f t="shared" si="4"/>
+        <v>1.3534478212312895E-4</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
@@ -5065,22 +5370,22 @@
       <c r="O61" s="7"/>
       <c r="P61" s="7"/>
       <c r="Q61" s="34">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="R61" s="7">
-        <v>239.48609999999999</v>
+        <v>240.14940000000001</v>
       </c>
       <c r="S61" s="24">
+        <f t="shared" si="5"/>
+        <v>261.89746639062406</v>
+      </c>
+      <c r="T61">
         <f t="shared" si="3"/>
-        <v>171.60367991761794</v>
-      </c>
-      <c r="T61">
-        <f t="shared" si="1"/>
-        <v>67.882420082382055</v>
+        <v>21.748066390624047</v>
       </c>
       <c r="U61">
-        <f t="shared" si="2"/>
-        <v>0.48459783847170745</v>
+        <f t="shared" si="4"/>
+        <v>1.0638634354727707E-4</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">
@@ -5095,22 +5400,22 @@
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="34">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="R62" s="7">
-        <v>238.85749999999999</v>
+        <v>239.48609999999999</v>
       </c>
       <c r="S62" s="24">
+        <f t="shared" si="5"/>
+        <v>261.8934014698284</v>
+      </c>
+      <c r="T62">
         <f t="shared" si="3"/>
-        <v>168.46151403444799</v>
-      </c>
-      <c r="T62">
-        <f t="shared" si="1"/>
-        <v>70.395985965552001</v>
+        <v>22.407301469828411</v>
       </c>
       <c r="U62">
-        <f t="shared" si="2"/>
-        <v>0.47567938561274464</v>
+        <f t="shared" si="4"/>
+        <v>8.3623867250846233E-5</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
@@ -5124,12 +5429,23 @@
       <c r="N63" s="7"/>
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
-      <c r="S63" s="26" t="s">
-        <v>25</v>
+      <c r="Q63" s="34">
+        <v>4</v>
+      </c>
+      <c r="R63" s="7">
+        <v>238.85749999999999</v>
+      </c>
+      <c r="S63" s="24">
+        <f t="shared" si="5"/>
+        <v>261.89017778206465</v>
       </c>
       <c r="T63">
-        <f>SUM(T3:T38)</f>
-        <v>136.34555898095485</v>
+        <f t="shared" si="3"/>
+        <v>23.032677782064667</v>
+      </c>
+      <c r="U63">
+        <f t="shared" si="4"/>
+        <v>6.5731661986104007E-5</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
@@ -5143,8 +5459,13 @@
       <c r="N64" s="7"/>
       <c r="O64" s="7"/>
       <c r="P64" s="7"/>
-      <c r="Q64" s="7"/>
-      <c r="R64" s="7"/>
+      <c r="S64" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="T64">
+        <f>SUM(T4:T39)</f>
+        <v>42.568659628743461</v>
+      </c>
     </row>
     <row r="65" spans="7:18" x14ac:dyDescent="0.2">
       <c r="G65" s="4"/>

</xml_diff>